<commit_message>
Fix: examples according to new rules
</commit_message>
<xml_diff>
--- a/files/test_files/Overall/Composicoes/composicoes_composition_teste.xlsx
+++ b/files/test_files/Overall/Composicoes/composicoes_composition_teste.xlsx
@@ -758,10 +758,10 @@
         <v>-1</v>
       </c>
       <c r="AD3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AE3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AF3">
         <v>-1</v>

</xml_diff>